<commit_message>
commit pour ma tour
</commit_message>
<xml_diff>
--- a/Event sheet sound design.xlsx
+++ b/Event sheet sound design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom99\Documents\GitHub\Phainiks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{804BB807-3564-40EA-865E-F3607CC89490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C990286-87A9-4A84-9029-0D9979BEEFBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{35707B74-11BD-4D6B-A632-19993C2BB170}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>EventName</t>
   </si>
@@ -79,31 +79,43 @@
     <t>Character</t>
   </si>
   <si>
-    <t>Environnement/ world</t>
-  </si>
-  <si>
-    <t>step</t>
-  </si>
-  <si>
-    <t>stop</t>
-  </si>
-  <si>
     <t>pick up items</t>
   </si>
   <si>
     <t>uses items</t>
   </si>
   <si>
-    <t>world change</t>
-  </si>
-  <si>
     <t>system</t>
   </si>
   <si>
     <t>reboot</t>
   </si>
   <si>
-    <t>²</t>
+    <t>click</t>
+  </si>
+  <si>
+    <t>walk</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>level start</t>
+  </si>
+  <si>
+    <t>level end</t>
+  </si>
+  <si>
+    <t>door open</t>
+  </si>
+  <si>
+    <t>end cycle</t>
+  </si>
+  <si>
+    <t>respawn</t>
+  </si>
+  <si>
+    <t>2d</t>
   </si>
 </sst>
 </file>
@@ -240,6 +252,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -254,9 +269,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D540DE7-AB5D-4544-93DA-8A026C25CA08}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,54 +596,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
@@ -656,50 +668,123 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -709,12 +794,12 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:P1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>